<commit_message>
add example env vars to localstack
</commit_message>
<xml_diff>
--- a/S3-files/example-template.xlsx
+++ b/S3-files/example-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
-  <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HoldingBrownB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BEBC8BD0-34DB-447C-9A40-AC518444AC4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF00413B-89EA-407C-B14C-D9088361D130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,6 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr/>
-    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -40,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Example sheet 1</t>
   </si>
@@ -54,7 +51,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -74,8 +71,8 @@
   </fills>
   <borders count="1">
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -104,7 +101,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -257,25 +254,25 @@
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110%"/>
-                <a:satMod val="105%"/>
-                <a:tint val="67%"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50%">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105%"/>
-                <a:satMod val="103%"/>
-                <a:tint val="73%"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100%">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105%"/>
-                <a:satMod val="109%"/>
-                <a:tint val="81%"/>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -283,25 +280,25 @@
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103%"/>
-                <a:lumMod val="102%"/>
-                <a:tint val="94%"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50%">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110%"/>
-                <a:lumMod val="100%"/>
-                <a:shade val="100%"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100%">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99%"/>
-                <a:satMod val="120%"/>
-                <a:shade val="78%"/>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -314,21 +311,21 @@
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800%"/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800%"/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800%"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -342,7 +339,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63%"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -354,32 +351,32 @@
         </a:solidFill>
         <a:solidFill>
           <a:schemeClr val="phClr">
-            <a:tint val="95%"/>
-            <a:satMod val="170%"/>
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
-              <a:schemeClr val="phClr">
-                <a:tint val="93%"/>
-                <a:satMod val="150%"/>
-                <a:shade val="98%"/>
-                <a:lumMod val="102%"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50%">
-              <a:schemeClr val="phClr">
-                <a:tint val="98%"/>
-                <a:satMod val="130%"/>
-                <a:shade val="90%"/>
-                <a:lumMod val="103%"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100%">
-              <a:schemeClr val="phClr">
-                <a:shade val="63%"/>
-                <a:satMod val="120%"/>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -399,7 +396,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -422,11 +419,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -442,10 +439,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>

</xml_diff>